<commit_message>
Added time to Quiz table of ER diagram
</commit_message>
<xml_diff>
--- a/OnlineQuizSchema.xlsx
+++ b/OnlineQuizSchema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="46">
   <si>
     <t>Field</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Data Dictionary of a quiz application</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="245901"/>
@@ -756,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G45"/>
+  <dimension ref="B3:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1002,93 +1008,90 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="17" t="s">
+      <c r="D21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>3</v>
@@ -1097,13 +1100,16 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>3</v>
@@ -1112,37 +1118,37 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>3</v>
+      <c r="F29" s="1">
+        <v>1</v>
       </c>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>30</v>
@@ -1157,7 +1163,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>30</v>
@@ -1172,7 +1178,7 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>30</v>
@@ -1185,162 +1191,177 @@
       </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="D34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
-    </row>
-    <row r="37" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="5" t="s">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
+      <c r="F39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="41" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
+      <c r="D40" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="42" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="16"/>
-    </row>
-    <row r="43" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="44" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="5" t="s">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+      <c r="F45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="10"/>
+      <c r="D46" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B37:G37"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>